<commit_message>
updated team info list and team folders
</commit_message>
<xml_diff>
--- a/healthcare_hackathon_teams_the netherlands.xlsx
+++ b/healthcare_hackathon_teams_the netherlands.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
   <si>
     <t>Team number:</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>JasperNederhoed@hotmail.com</t>
+  </si>
+  <si>
+    <t>Dermatology companion app.</t>
+  </si>
+  <si>
+    <t>Skin cancer data set</t>
   </si>
 </sst>
 </file>
@@ -991,7 +997,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,10 +1061,16 @@
       <c r="A9" t="s">
         <v>3</v>
       </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
team 2 information updated
</commit_message>
<xml_diff>
--- a/healthcare_hackathon_teams_the netherlands.xlsx
+++ b/healthcare_hackathon_teams_the netherlands.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Team number:</t>
   </si>
@@ -108,9 +108,6 @@
     <t>girindra.wardhan@gmail.com</t>
   </si>
   <si>
-    <t>https://nl.linkedin.com/in/girindrawardhana</t>
-  </si>
-  <si>
     <t>Yani Mandasari</t>
   </si>
   <si>
@@ -217,6 +214,15 @@
   </si>
   <si>
     <t>Skin cancer data set</t>
+  </si>
+  <si>
+    <t>Cloud-based skin cancer prediction, for anyone, anytime, anywhere</t>
+  </si>
+  <si>
+    <t>ISIC skin lesion dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.linkedin.com/in/girindrawardhana </t>
   </si>
 </sst>
 </file>
@@ -691,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,51 +746,57 @@
       <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
-        <v>28</v>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -836,6 +848,7 @@
     <hyperlink ref="D5" r:id="rId7"/>
     <hyperlink ref="C7" r:id="rId8"/>
     <hyperlink ref="D7" r:id="rId9"/>
+    <hyperlink ref="D4" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -870,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -878,57 +891,57 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -996,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1021,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1029,32 +1042,32 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1062,7 +1075,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1070,7 +1083,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
excel file of teams updated
</commit_message>
<xml_diff>
--- a/healthcare_hackathon_teams_the netherlands.xlsx
+++ b/healthcare_hackathon_teams_the netherlands.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
   <si>
     <t>Team number:</t>
   </si>
@@ -223,6 +223,33 @@
   </si>
   <si>
     <t xml:space="preserve">https://nl.linkedin.com/in/girindrawardhana </t>
+  </si>
+  <si>
+    <t>End (Amsterdam time):</t>
+  </si>
+  <si>
+    <t>09:30 Sunday (Deadline was 10:00 due to Summer time shift)</t>
+  </si>
+  <si>
+    <t>09:00 Saturday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://surfdrive.surf.nl/files/index.php/s/XDqe1jx5GETaf4X </t>
+  </si>
+  <si>
+    <t>Everything is complete under:</t>
+  </si>
+  <si>
+    <t>https://youtu.be/wijWW5HopG0</t>
+  </si>
+  <si>
+    <t>CODE DEMO video:</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ZnxV_MA78os</t>
+  </si>
+  <si>
+    <t>https://github.com/bsirmacek/SchoolofAI_Healthcare_Hackathon_the_Netherlands/tree/master/Team2_Lotad.AI_completed</t>
   </si>
 </sst>
 </file>
@@ -254,12 +281,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -275,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -283,6 +316,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -695,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,7 +759,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="5">
         <v>2</v>
       </c>
     </row>
@@ -800,41 +846,80 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4">
-        <v>0.375</v>
+      <c r="B11" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B15" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B16" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B17" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B18" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>10</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -849,8 +934,16 @@
     <hyperlink ref="C7" r:id="rId8"/>
     <hyperlink ref="D7" r:id="rId9"/>
     <hyperlink ref="D4" r:id="rId10"/>
+    <hyperlink ref="B15" r:id="rId11" display="https://surfdrive.surf.nl/files/index.php/s/XDqe1jx5GETaf4X"/>
+    <hyperlink ref="B16" r:id="rId12" display="https://surfdrive.surf.nl/files/index.php/s/XDqe1jx5GETaf4X"/>
+    <hyperlink ref="B17" r:id="rId13" display="https://surfdrive.surf.nl/files/index.php/s/XDqe1jx5GETaf4X"/>
+    <hyperlink ref="B18" r:id="rId14" display="https://surfdrive.surf.nl/files/index.php/s/XDqe1jx5GETaf4X"/>
+    <hyperlink ref="B19" r:id="rId15"/>
+    <hyperlink ref="B20" r:id="rId16"/>
+    <hyperlink ref="B14" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>